<commit_message>
excel for test cases and validation
</commit_message>
<xml_diff>
--- a/Test cases.xlsx
+++ b/Test cases.xlsx
@@ -8,13 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\SDET\RESTful Booker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E325443-3A22-4DD6-AF90-A57A4787DE46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B052FD48-0FA2-4463-897F-111A04EA1626}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{8FA8426C-5C8A-4061-B831-E647FE9F19BC}"/>
   </bookViews>
   <sheets>
     <sheet name="Auth" sheetId="1" r:id="rId1"/>
     <sheet name="Booking" sheetId="2" r:id="rId2"/>
+    <sheet name="Ping" sheetId="3" r:id="rId3"/>
+    <sheet name="Variables" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="69">
   <si>
     <t>TCID</t>
   </si>
@@ -88,65 +90,273 @@
     <t>None</t>
   </si>
   <si>
+    <t>https://restful-booker.herokuapp.com/</t>
+  </si>
+  <si>
+    <t>Content-Type: application/json</t>
+  </si>
+  <si>
+    <t>Auth tokens needs to be generated</t>
+  </si>
+  <si>
+    <t>Get Booking IDs</t>
+  </si>
+  <si>
+    <t>Fetch all Booking Ids</t>
+  </si>
+  <si>
+    <t>GET</t>
+  </si>
+  <si>
+    <t>{{baseURL}}booking</t>
+  </si>
+  <si>
+    <t>baseURL</t>
+  </si>
+  <si>
+    <t>Collection Variable</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>Booking</t>
+  </si>
+  <si>
+    <t>token</t>
+  </si>
+  <si>
+    <t>skipCollectionTests</t>
+  </si>
+  <si>
+    <t>{{baseURL}}ping</t>
+  </si>
+  <si>
+    <t>Check Health Status</t>
+  </si>
+  <si>
+    <t>Need to ping server to check the health status</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Created</t>
+  </si>
+  <si>
+    <t>Status code is 201
+Content Type is present in Response Header
+Content type should be text/plain</t>
+  </si>
+  <si>
+    <t>Status code is 200
+token field should be non-empty
+Content type is application/json</t>
+  </si>
+  <si>
     <t>{
-    "username" : {{username}},
-    "password" : {{password}}
+    "username" : "admin",
+    "password" : "password123"
 }</t>
   </si>
   <si>
-    <t>Should return Token String</t>
-  </si>
-  <si>
-    <t>Status code
-token field should be non-empty</t>
-  </si>
-  <si>
-    <t>https://restful-booker.herokuapp.com/</t>
-  </si>
-  <si>
-    <t>Content-Type: application/json</t>
-  </si>
-  <si>
-    <t>Auth tokens needs to be generated</t>
-  </si>
-  <si>
-    <t>Get Booking IDs</t>
-  </si>
-  <si>
-    <t>Fetch all Booking Ids</t>
-  </si>
-  <si>
-    <t>Fetch Bookings Ids filtered using username</t>
-  </si>
-  <si>
-    <t>Fetch Booking Ids filtered using check-in and check-out dates</t>
-  </si>
-  <si>
-    <t>GET</t>
-  </si>
-  <si>
-    <t>{{baseURL}}</t>
-  </si>
-  <si>
-    <t>{{baseURL}}booking</t>
+    <t>Get Booking Details by ID</t>
+  </si>
+  <si>
+    <t>Create Booking</t>
+  </si>
+  <si>
+    <t>Get the created Booking</t>
+  </si>
+  <si>
+    <t>Update the booking</t>
+  </si>
+  <si>
+    <t>Delete the booking</t>
+  </si>
+  <si>
+    <t>PUT</t>
+  </si>
+  <si>
+    <t>DELETE</t>
+  </si>
+  <si>
+    <t>{{token}}</t>
+  </si>
+  <si>
+    <t>Content-Type: application/json
+Cookie: token={{token}}</t>
+  </si>
+  <si>
+    <t>{{baseURL}}booking/{{id}}</t>
+  </si>
+  <si>
+    <t>bookingID</t>
+  </si>
+  <si>
+    <t>{{baseURL}}booking/{{bookingId}}</t>
+  </si>
+  <si>
+    <t>{
+    "token": "24777a1a141beaf"
+}</t>
+  </si>
+  <si>
+    <t>Fetch specific booking details using booking ID</t>
+  </si>
+  <si>
+    <t>Create a booking request</t>
+  </si>
+  <si>
+    <t>Fetch the created booking</t>
+  </si>
+  <si>
+    <t>Update the created booking</t>
+  </si>
+  <si>
+    <t>Delete the created booking</t>
+  </si>
+  <si>
+    <t>[
+    {
+        "bookingid": 8
+    },
+    {
+        "bookingid": 548
+    },
+    {
+        "bookingid": 2142
+    },
+    {
+        "bookingid": 780
+    },
+    {
+        "bookingid": 2168
+    },
+    {
+        "bookingid": 977
+    },</t>
+  </si>
+  <si>
+    <t>{
+    "firstname": "firstnamePatch",
+    "lastname": "lastnamePatch",
+    "totalprice": 111,
+    "depositpaid": true,
+    "bookingdates": {
+        "checkin": "2018-01-01",
+        "checkout": "2019-01-01"
+    },
+    "additionalneeds": "Breakfast"
+}</t>
+  </si>
+  <si>
+    <t>{
+    "bookingid": 2906,
+    "booking": {
+        "firstname": "Tejas",
+        "lastname": "Bansal",
+        "totalprice": 111,
+        "depositpaid": true,
+        "bookingdates": {
+            "checkin": "2025-01-01",
+            "checkout": "2025-01-08"
+        },
+        "additionalneeds": "Breakfast"
+    }
+}</t>
+  </si>
+  <si>
+    <t>{
+    "firstname" : "Tejas",
+    "lastname" : "Bansal",
+    "totalprice" : 111,
+    "depositpaid" : true,
+    "bookingdates" : {
+        "checkin" : "2025-01-01",
+        "checkout" : "2025-01-08"
+    },
+    "additionalneeds" : "Breakfast"
+}</t>
+  </si>
+  <si>
+    <t>{
+    "firstname": "Tejas",
+    "lastname": "Bansal",
+    "totalprice": 111,
+    "depositpaid": true,
+    "bookingdates": {
+        "checkin": "2025-01-01",
+        "checkout": "2025-01-08"
+    },
+    "additionalneeds": "Breakfast"
+}</t>
+  </si>
+  <si>
+    <t>{
+    "firstname" : "Tejas",
+    "lastname" : "Bansal",
+    "totalprice" : 111,
+    "depositpaid" : true,
+    "bookingdates" : {
+        "checkin" : "2025-01-01",
+        "checkout" : "2025-01-10"
+    },
+    "additionalneeds" : "Lunch"
+}</t>
+  </si>
+  <si>
+    <t>{
+    "firstname": "Tejas",
+    "lastname": "Bansal",
+    "totalprice": 111,
+    "depositpaid": true,
+    "bookingdates": {
+        "checkin": "2025-01-01",
+        "checkout": "2025-01-10"
+    },
+    "additionalneeds": "Lunch"
+}</t>
+  </si>
+  <si>
+    <t>Validate status code
+Response Array should not be empty
+Each entry should have unique booking ID
+Each id is a number</t>
+  </si>
+  <si>
+    <t>Validate status code
+Validate response schema
+Validate by giving invalid id</t>
+  </si>
+  <si>
+    <t>Validate status code
+Validate response schema
+Verifying using invalid data
+Booking ID should not be null</t>
+  </si>
+  <si>
+    <t>Validate status code
+Validate response schema</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Validate status code
+Content type
+Validate response schema
+</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -169,8 +379,37 @@
       <name val="Consolas"/>
       <family val="3"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -183,8 +422,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0070C0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -222,38 +467,67 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -568,8 +842,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B42CAD9-668F-44A3-B246-302C873D14B3}">
   <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView topLeftCell="I1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -583,90 +857,90 @@
     <col min="7" max="7" width="17.77734375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="16.6640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="38.5546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="23.5546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="32.44140625" customWidth="1"/>
+    <col min="11" max="11" width="31.77734375" customWidth="1"/>
     <col min="12" max="12" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="55.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K1" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="L1" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="M1" s="12" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="87" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3" t="s">
+    <row r="2" spans="1:13" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="13"/>
+      <c r="B2" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D2" s="3" t="s">
+      <c r="C2" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="F2" s="3" t="s">
+      <c r="E2" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="I2" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="J2" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="K2" s="3" t="s">
+      <c r="I2" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="L2" s="3">
+      <c r="J2" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="K2" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="L2" s="13">
         <v>200</v>
       </c>
-      <c r="M2" s="5" t="s">
-        <v>19</v>
+      <c r="M2" s="14" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -676,213 +950,311 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CF4D02B-A25C-4B68-BA90-439DA48B009D}">
-  <dimension ref="A1:M13"/>
+  <dimension ref="A1:M14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="5.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.77734375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="44.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.5546875" customWidth="1"/>
+    <col min="5" max="5" width="43" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="29.109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="17" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="16" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="26.6640625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="21.77734375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="29.88671875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="35.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H1" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="I1" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="J1" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="K1" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="6" t="s">
+      <c r="L1" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="M1" s="16" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1" t="s">
+    <row r="2" spans="1:13" ht="274.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="11"/>
+      <c r="B2" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1"/>
-    </row>
-    <row r="3" spans="1:13" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1" t="s">
+      <c r="G2" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="H2" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="I2" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="J2" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="K2" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="L2" s="11">
+        <v>200</v>
+      </c>
+      <c r="M2" s="11" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="159" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="11"/>
+      <c r="B3" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="G3" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="H3" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="I3" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="J3" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="K3" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="L3" s="11">
+        <v>200</v>
+      </c>
+      <c r="M3" s="11" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="288.60000000000002" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="11"/>
+      <c r="B4" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
-      <c r="K3" s="1"/>
-      <c r="L3" s="1"/>
-      <c r="M3" s="1"/>
-    </row>
-    <row r="4" spans="1:13" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
-      <c r="K4" s="1"/>
-      <c r="L4" s="1"/>
-      <c r="M4" s="1"/>
-    </row>
-    <row r="5" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
-      <c r="K5" s="1"/>
-      <c r="L5" s="1"/>
-      <c r="M5" s="1"/>
-    </row>
-    <row r="6" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
-      <c r="K6" s="1"/>
-      <c r="L6" s="1"/>
-      <c r="M6" s="1"/>
-    </row>
-    <row r="7" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
-      <c r="K7" s="1"/>
-      <c r="L7" s="1"/>
-      <c r="M7" s="1"/>
-    </row>
-    <row r="8" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G4" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="H4" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="I4" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="J4" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="K4" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="L4" s="11">
+        <v>200</v>
+      </c>
+      <c r="M4" s="11" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="159" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="11"/>
+      <c r="B5" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="G5" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="H5" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="I5" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="J5" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="K5" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="L5" s="11">
+        <v>200</v>
+      </c>
+      <c r="M5" s="11" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="288.60000000000002" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="11"/>
+      <c r="B6" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="E6" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="F6" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="G6" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="H6" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="I6" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="J6" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="K6" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="L6" s="11">
+        <v>200</v>
+      </c>
+      <c r="M6" s="11" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="11"/>
+      <c r="B7" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="E7" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="F7" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="G7" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="H7" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="I7" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="J7" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="K7" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="L7" s="11">
+        <v>201</v>
+      </c>
+      <c r="M7" s="11" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
-      <c r="E8" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>28</v>
-      </c>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
@@ -891,17 +1263,13 @@
       <c r="L8" s="1"/>
       <c r="M8" s="1"/>
     </row>
-    <row r="9" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
-      <c r="E9" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>28</v>
-      </c>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
@@ -910,17 +1278,13 @@
       <c r="L9" s="1"/>
       <c r="M9" s="1"/>
     </row>
-    <row r="10" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
-      <c r="E10" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>28</v>
-      </c>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
@@ -929,17 +1293,13 @@
       <c r="L10" s="1"/>
       <c r="M10" s="1"/>
     </row>
-    <row r="11" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
-      <c r="E11" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>28</v>
-      </c>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
@@ -948,48 +1308,275 @@
       <c r="L11" s="1"/>
       <c r="M11" s="1"/>
     </row>
-    <row r="12" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="D12" s="1"/>
-      <c r="E12" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="F12" s="1" t="s">
+      <c r="E12" s="1"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDDDBDDC-A1EF-46B5-84F7-7D4F83E90053}">
+  <dimension ref="A1:M6"/>
+  <sheetViews>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="L9" sqref="L9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="43" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.21875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.21875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="28.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="10"/>
+      <c r="B2" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="H2" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="I2" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="J2" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="K2" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="L2" s="10">
+        <v>201</v>
+      </c>
+      <c r="M2" s="11" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="E6" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{274CC7E3-3EF1-4E5F-805B-C33BD4651FA2}">
+  <dimension ref="D2:H21"/>
+  <sheetViews>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="4" max="4" width="18.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="41.21875" customWidth="1"/>
+    <col min="6" max="6" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="33.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+    </row>
+    <row r="3" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+    </row>
+    <row r="4" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+    </row>
+    <row r="5" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+    </row>
+    <row r="7" spans="4:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D7" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
-      <c r="J12" s="1"/>
-      <c r="K12" s="1"/>
-      <c r="L12" s="1"/>
-      <c r="M12" s="1"/>
-    </row>
-    <row r="13" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
-      <c r="I13" s="1"/>
-      <c r="J13" s="1"/>
-      <c r="K13" s="1"/>
-      <c r="L13" s="1"/>
-      <c r="M13" s="1"/>
+      <c r="E7" s="2"/>
+    </row>
+    <row r="8" spans="4:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D8" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="4:8" s="3" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D9" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="4:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D10" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E10" s="4"/>
+    </row>
+    <row r="11" spans="4:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D11" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E11" s="4"/>
+    </row>
+    <row r="12" spans="4:8" s="6" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D12" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="E12" s="7"/>
+    </row>
+    <row r="13" spans="4:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D13" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E13" s="4"/>
+    </row>
+    <row r="14" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+    </row>
+    <row r="15" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+    </row>
+    <row r="16" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+    </row>
+    <row r="17" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+    </row>
+    <row r="18" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+    </row>
+    <row r="19" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+    </row>
+    <row r="20" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+    </row>
+    <row r="21" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="E3" r:id="rId1" xr:uid="{19CD44A6-59E2-448A-9D95-0F8A08342C45}"/>
-  </hyperlinks>
+  <mergeCells count="1">
+    <mergeCell ref="D7:E7"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>